<commit_message>
Updated title on map
</commit_message>
<xml_diff>
--- a/newspaper contacts.xlsx
+++ b/newspaper contacts.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEEF7F7-DF21-4745-8885-C54141A3FF27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Doug Brown</t>
   </si>
@@ -83,12 +82,66 @@
   </si>
   <si>
     <t>info@EatDrinkBoulder.com</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>New Denizen</t>
+  </si>
+  <si>
+    <t>newdenizenblog@gmail.com</t>
+  </si>
+  <si>
+    <t>food blogger</t>
+  </si>
+  <si>
+    <t>Josie Sexton</t>
+  </si>
+  <si>
+    <t>Eater Denver</t>
+  </si>
+  <si>
+    <t>https://www.josiesexton.com/contact.html</t>
+  </si>
+  <si>
+    <t>Food blogger at multiple organizations (was at the Coloradoan in the past?)</t>
+  </si>
+  <si>
+    <t>milehighandhungry@gmail.com</t>
+  </si>
+  <si>
+    <t>http://milehighandhungry.com/</t>
+  </si>
+  <si>
+    <t>Instagram influencer and blogger</t>
+  </si>
+  <si>
+    <t>They have a favorite hh spot</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/bestboozedenver/</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/Denverfoodscene/</t>
+  </si>
+  <si>
+    <t>Has already posted about an app</t>
+  </si>
+  <si>
+    <t>Cara Chancellor</t>
+  </si>
+  <si>
+    <t>cara.chancellor@yahoo.com</t>
+  </si>
+  <si>
+    <t>303 magazine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,16 +477,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -467,7 +526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -475,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -489,12 +548,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -505,7 +564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
@@ -513,11 +572,82 @@
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C8CCB7FD-3DB4-4C52-A371-045BA9E608D3}"/>
-    <hyperlink ref="C3" r:id="rId2" display="mailto:nibbles@boulderweekly.com" xr:uid="{F347957E-3B0D-4AE9-82BD-90B90DC6DC8C}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{2545BB4A-C5AF-4C9B-8F4A-570571B5F87F}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2" display="mailto:nibbles@boulderweekly.com"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5" display="mailto:milehighandhungry@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>